<commit_message>
added ap work for this week
</commit_message>
<xml_diff>
--- a/ap projects/APCurriculum/currMatrixScoreCard.xlsx
+++ b/ap projects/APCurriculum/currMatrixScoreCard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr. Neato\Desktop\github\T21\ap projects\APCurriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CF4FDC-22B5-4D7A-98B6-1A50DCB16332}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7BDB8-5D1E-4039-9B81-0F8676319230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="1440" windowWidth="23430" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3885" yWindow="1275" windowWidth="23430" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>Using the Math Class</t>
   </si>
   <si>
-    <t>T21 014, 056, 069, 087, 088, 089, 090</t>
-  </si>
-  <si>
     <t>Unit 3 - Boolean Expressions &amp; If Statements</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>Creating Superclasses &amp; Subclasses</t>
   </si>
   <si>
-    <t>T21 098, 099</t>
-  </si>
-  <si>
     <t>Writing Constructors for Subclasses</t>
   </si>
   <si>
@@ -368,6 +362,12 @@
   </si>
   <si>
     <t xml:space="preserve">T21 016, 017, 018, 084 </t>
+  </si>
+  <si>
+    <t>T21 014, 056, 069, 087</t>
+  </si>
+  <si>
+    <t>T21 095, 098, 099</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -471,6 +471,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -850,8 +851,8 @@
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>28</v>
+      <c r="B19" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C19" s="12">
         <v>44214</v>
@@ -862,7 +863,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3"/>
     </row>
@@ -871,55 +872,55 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="C28" s="5"/>
     </row>
@@ -928,7 +929,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C30" s="5"/>
     </row>
@@ -937,10 +938,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C32" s="10">
         <v>44214</v>
@@ -948,10 +949,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="C33" s="10">
         <v>44214</v>
@@ -959,10 +960,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="C34" s="10">
         <v>44207</v>
@@ -970,19 +971,19 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C36" s="5"/>
     </row>
@@ -991,7 +992,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" s="3"/>
     </row>
@@ -1000,91 +1001,91 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C44" s="3"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="C48" s="3"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="C49" s="3"/>
     </row>
@@ -1093,7 +1094,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C51" s="3"/>
     </row>
@@ -1102,37 +1103,37 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="C54" s="3"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" s="9" t="s">
         <v>77</v>
-      </c>
-      <c r="B56" s="9" t="s">
-        <v>78</v>
       </c>
       <c r="C56" s="3"/>
     </row>
@@ -1141,7 +1142,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C58" s="3"/>
     </row>
@@ -1150,7 +1151,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60" s="8" t="s">
         <v>26</v>
@@ -1159,7 +1160,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="8" t="s">
         <v>26</v>
@@ -1168,46 +1169,46 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>83</v>
       </c>
       <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>84</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="C63" s="3"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B64" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>87</v>
       </c>
       <c r="C64" s="3"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="3"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="C66" s="3"/>
     </row>
@@ -1216,7 +1217,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C68" s="3"/>
     </row>
@@ -1225,19 +1226,19 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B70" s="8" t="s">
         <v>92</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="C70" s="3"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C71" s="3"/>
     </row>
@@ -1246,7 +1247,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C73" s="3"/>
     </row>
@@ -1255,64 +1256,70 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="C75" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="C75" s="12">
+        <v>44228</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C76" s="3"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C78" s="3"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C79" s="3"/>
+        <v>102</v>
+      </c>
+      <c r="C79" s="12">
+        <v>44228</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C80" s="3"/>
+        <v>104</v>
+      </c>
+      <c r="C80" s="12">
+        <v>44228</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>106</v>
       </c>
       <c r="C81" s="12">
         <v>44221</v>
@@ -1323,7 +1330,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C83" s="3"/>
     </row>
@@ -1332,19 +1339,19 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C86" s="3"/>
     </row>

</xml_diff>

<commit_message>
added 097 lab for AP
</commit_message>
<xml_diff>
--- a/ap projects/APCurriculum/currMatrixScoreCard.xlsx
+++ b/ap projects/APCurriculum/currMatrixScoreCard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr. Neato\Desktop\github\T21\ap projects\APCurriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7BDB8-5D1E-4039-9B81-0F8676319230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE3138B-E155-492E-8855-B7A62B5B947C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="1275" windowWidth="23430" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="1365" windowWidth="23430" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1272,9 @@
       <c r="B76" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="3"/>
+      <c r="C76" s="12">
+        <v>44236</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
@@ -1281,7 +1283,9 @@
       <c r="B77" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="3"/>
+      <c r="C77" s="12">
+        <v>44236</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
@@ -1290,7 +1294,9 @@
       <c r="B78" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C78" s="3"/>
+      <c r="C78" s="12">
+        <v>44236</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">

</xml_diff>

<commit_message>
added first assignment for ap
</commit_message>
<xml_diff>
--- a/ap projects/APCurriculum/currMatrixScoreCard.xlsx
+++ b/ap projects/APCurriculum/currMatrixScoreCard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr. Neato\Desktop\github\T21\ap projects\APCurriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE3138B-E155-492E-8855-B7A62B5B947C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7FA3FA-651B-49D4-A26F-38BF745195F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1365" windowWidth="23430" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2220" windowWidth="25245" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1258,7 +1258,7 @@
       <c r="A75" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="8" t="s">
+      <c r="B75" s="14" t="s">
         <v>115</v>
       </c>
       <c r="C75" s="12">
@@ -1269,7 +1269,7 @@
       <c r="A76" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="14" t="s">
         <v>97</v>
       </c>
       <c r="C76" s="12">
@@ -1280,7 +1280,7 @@
       <c r="A77" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B77" s="8" t="s">
+      <c r="B77" s="14" t="s">
         <v>99</v>
       </c>
       <c r="C77" s="12">
@@ -1291,7 +1291,7 @@
       <c r="A78" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="14" t="s">
         <v>99</v>
       </c>
       <c r="C78" s="12">
@@ -1306,14 +1306,14 @@
         <v>102</v>
       </c>
       <c r="C79" s="12">
-        <v>44228</v>
+        <v>44243</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="B80" s="14" t="s">
         <v>104</v>
       </c>
       <c r="C80" s="12">

</xml_diff>

<commit_message>
added ArrayList to ap
</commit_message>
<xml_diff>
--- a/ap projects/APCurriculum/currMatrixScoreCard.xlsx
+++ b/ap projects/APCurriculum/currMatrixScoreCard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr. Neato\Desktop\github\T21\ap projects\APCurriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7FA3FA-651B-49D4-A26F-38BF745195F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0412F4B1-DD6C-4A51-B214-097B66E2B6E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2220" windowWidth="25245" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,7 +693,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H61" sqref="H61"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -845,7 +845,9 @@
       <c r="B18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="12">
+        <v>44243</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
@@ -1156,7 +1158,9 @@
       <c r="B60" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="3"/>
+      <c r="C60" s="12">
+        <v>44243</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
@@ -1165,7 +1169,9 @@
       <c r="B61" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="12">
+        <v>44243</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">

</xml_diff>

<commit_message>
update ap curriculum matrix
</commit_message>
<xml_diff>
--- a/ap projects/APCurriculum/currMatrixScoreCard.xlsx
+++ b/ap projects/APCurriculum/currMatrixScoreCard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr. Neato\Desktop\github\T21\ap projects\APCurriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DC000C-E5A8-4744-A241-26FF22CA5C7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166BD8C7-A540-42DA-9AAB-A5050910A404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1785" windowWidth="25350" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2220" windowWidth="22755" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -692,8 +692,8 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -751,7 +751,9 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="10">
+        <v>44278</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1208,7 +1210,7 @@
       <c r="A65" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="8" t="s">
+      <c r="B65" s="14" t="s">
         <v>86</v>
       </c>
       <c r="C65" s="12">
@@ -1362,7 +1364,9 @@
       <c r="B85" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C85" s="3"/>
+      <c r="C85" s="12">
+        <v>44278</v>
+      </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
@@ -1371,7 +1375,9 @@
       <c r="B86" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C86" s="3"/>
+      <c r="C86" s="12">
+        <v>44278</v>
+      </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C87" s="3"/>

</xml_diff>

<commit_message>
added ap curr update
</commit_message>
<xml_diff>
--- a/ap projects/APCurriculum/currMatrixScoreCard.xlsx
+++ b/ap projects/APCurriculum/currMatrixScoreCard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dr. Neato\Desktop\github\T21\ap projects\APCurriculum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166BD8C7-A540-42DA-9AAB-A5050910A404}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C82B969-69D6-46C0-B23F-093550FF95D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2220" windowWidth="22755" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26775" windowHeight="13380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +433,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -455,7 +461,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -472,6 +477,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -748,10 +754,10 @@
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>44278</v>
       </c>
     </row>
@@ -759,10 +765,10 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <v>44207</v>
       </c>
     </row>
@@ -833,10 +839,10 @@
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>44207</v>
       </c>
     </row>
@@ -844,10 +850,10 @@
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>44243</v>
       </c>
     </row>
@@ -855,10 +861,10 @@
       <c r="A19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>44214</v>
       </c>
     </row>
@@ -908,46 +914,48 @@
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="5"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="5"/>
+      <c r="C27" s="9">
+        <v>44284</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="5"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C29" s="5"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C31" s="5"/>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="10">
+      <c r="C32" s="9">
         <v>44214</v>
       </c>
     </row>
@@ -955,10 +963,10 @@
       <c r="A33" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="10">
+      <c r="C33" s="9">
         <v>44214</v>
       </c>
     </row>
@@ -966,10 +974,10 @@
       <c r="A34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <v>44207</v>
       </c>
     </row>
@@ -980,16 +988,16 @@
       <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="5"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C37" s="3"/>
@@ -1025,7 +1033,7 @@
       <c r="A42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>54</v>
       </c>
       <c r="C42" s="3"/>
@@ -1061,7 +1069,7 @@
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C46" s="3"/>
@@ -1079,7 +1087,7 @@
       <c r="A48" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>66</v>
       </c>
       <c r="C48" s="3"/>
@@ -1088,7 +1096,7 @@
       <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C49" s="3"/>
@@ -1118,7 +1126,7 @@
       <c r="A54" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="8" t="s">
         <v>73</v>
       </c>
       <c r="C54" s="3"/>
@@ -1136,7 +1144,7 @@
       <c r="A56" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="8" t="s">
         <v>77</v>
       </c>
       <c r="C56" s="3"/>
@@ -1157,10 +1165,10 @@
       <c r="A60" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C60" s="12">
+      <c r="C60" s="11">
         <v>44243</v>
       </c>
     </row>
@@ -1168,10 +1176,10 @@
       <c r="A61" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C61" s="12">
+      <c r="C61" s="11">
         <v>44243</v>
       </c>
     </row>
@@ -1179,10 +1187,10 @@
       <c r="A62" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="12">
+      <c r="C62" s="11">
         <v>44249</v>
       </c>
     </row>
@@ -1190,10 +1198,10 @@
       <c r="A63" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C63" s="12">
+      <c r="C63" s="11">
         <v>44249</v>
       </c>
     </row>
@@ -1201,19 +1209,19 @@
       <c r="A64" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B64" s="8" t="s">
+      <c r="B64" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C64" s="12"/>
+      <c r="C64" s="11"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="12">
+      <c r="C65" s="11">
         <v>44263</v>
       </c>
     </row>
@@ -1221,7 +1229,7 @@
       <c r="A66" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C66" s="3"/>
@@ -1242,19 +1250,23 @@
       <c r="A70" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B70" s="8" t="s">
+      <c r="B70" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C70" s="3"/>
+      <c r="C70" s="11">
+        <v>44291</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B71" s="8" t="s">
+      <c r="B71" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="3"/>
+      <c r="C71" s="11">
+        <v>44291</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C72" s="3"/>
@@ -1272,10 +1284,10 @@
       <c r="A75" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="C75" s="12">
+      <c r="C75" s="11">
         <v>44228</v>
       </c>
     </row>
@@ -1283,10 +1295,10 @@
       <c r="A76" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="C76" s="12">
+      <c r="C76" s="11">
         <v>44236</v>
       </c>
     </row>
@@ -1294,10 +1306,10 @@
       <c r="A77" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C77" s="12">
+      <c r="C77" s="11">
         <v>44236</v>
       </c>
     </row>
@@ -1305,10 +1317,10 @@
       <c r="A78" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="C78" s="12">
+      <c r="C78" s="11">
         <v>44236</v>
       </c>
     </row>
@@ -1316,10 +1328,10 @@
       <c r="A79" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C79" s="12">
+      <c r="C79" s="11">
         <v>44243</v>
       </c>
     </row>
@@ -1327,10 +1339,10 @@
       <c r="A80" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="C80" s="12">
+      <c r="C80" s="11">
         <v>44228</v>
       </c>
     </row>
@@ -1338,10 +1350,10 @@
       <c r="A81" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="C81" s="12">
+      <c r="C81" s="11">
         <v>44221</v>
       </c>
     </row>
@@ -1361,10 +1373,10 @@
       <c r="A85" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="B85" s="8" t="s">
+      <c r="B85" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="C85" s="12">
+      <c r="C85" s="11">
         <v>44278</v>
       </c>
     </row>
@@ -1372,10 +1384,10 @@
       <c r="A86" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="B86" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="C86" s="12">
+      <c r="C86" s="11">
         <v>44278</v>
       </c>
     </row>

</xml_diff>